<commit_message>
Fix: updated server-side changes
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="112">
   <si>
     <t>Order ID</t>
   </si>
@@ -142,6 +142,18 @@
     <t>HK1033</t>
   </si>
   <si>
+    <t>HK1034</t>
+  </si>
+  <si>
+    <t>HK1035</t>
+  </si>
+  <si>
+    <t>HK1036</t>
+  </si>
+  <si>
+    <t>HK1037</t>
+  </si>
+  <si>
     <t>12/03/2025</t>
   </si>
   <si>
@@ -166,6 +178,9 @@
     <t>12/12/2025</t>
   </si>
   <si>
+    <t>12/16/2025</t>
+  </si>
+  <si>
     <t>Gowri</t>
   </si>
   <si>
@@ -220,6 +235,12 @@
     <t>Hemanth</t>
   </si>
   <si>
+    <t>Sunitha Woodlands</t>
+  </si>
+  <si>
+    <t>Shalini Raju</t>
+  </si>
+  <si>
     <t>Dosa Batter with Chutney</t>
   </si>
   <si>
@@ -311,6 +332,15 @@
   </si>
   <si>
     <t>Tandoori Chicken Biriyani</t>
+  </si>
+  <si>
+    <t>Dosa Batter</t>
+  </si>
+  <si>
+    <t>Veg Curries</t>
+  </si>
+  <si>
+    <t>Boiled egg curry with Jeera rice</t>
   </si>
   <si>
     <t>Delivered</t>
@@ -681,7 +711,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,13 +748,13 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -736,7 +766,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -744,13 +774,13 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -762,7 +792,7 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -770,13 +800,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -788,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -796,13 +826,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -814,7 +844,7 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -822,13 +852,13 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -840,7 +870,7 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -848,13 +878,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -866,7 +896,7 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -874,13 +904,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -892,7 +922,7 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -900,13 +930,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -918,7 +948,7 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -926,13 +956,13 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -944,7 +974,7 @@
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -952,13 +982,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -970,7 +1000,7 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -978,13 +1008,13 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -996,7 +1026,7 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1004,13 +1034,13 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E13">
         <v>15</v>
@@ -1022,7 +1052,7 @@
         <v>45</v>
       </c>
       <c r="H13" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1030,13 +1060,13 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -1048,7 +1078,7 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1056,13 +1086,13 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -1074,7 +1104,7 @@
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1082,13 +1112,13 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -1100,7 +1130,7 @@
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1108,13 +1138,13 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E17">
         <v>20</v>
@@ -1126,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1134,13 +1164,13 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -1152,7 +1182,7 @@
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1163,10 +1193,10 @@
         <v>45995</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E19">
         <v>30</v>
@@ -1178,7 +1208,7 @@
         <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1186,13 +1216,13 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E20">
         <v>10</v>
@@ -1204,7 +1234,7 @@
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1212,13 +1242,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E21">
         <v>10</v>
@@ -1230,7 +1260,7 @@
         <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1238,13 +1268,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -1256,7 +1286,7 @@
         <v>30</v>
       </c>
       <c r="H22" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1264,13 +1294,13 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -1282,7 +1312,7 @@
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1290,13 +1320,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E24">
         <v>10</v>
@@ -1308,7 +1338,7 @@
         <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1316,13 +1346,13 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E25">
         <v>80</v>
@@ -1334,7 +1364,7 @@
         <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1342,13 +1372,13 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E26">
         <v>120</v>
@@ -1360,7 +1390,7 @@
         <v>120</v>
       </c>
       <c r="H26" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1368,13 +1398,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -1386,7 +1416,7 @@
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1394,13 +1424,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E28">
         <v>20</v>
@@ -1412,7 +1442,7 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1420,13 +1450,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1438,7 +1468,7 @@
         <v>30</v>
       </c>
       <c r="H29" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1446,13 +1476,13 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -1464,7 +1494,7 @@
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1472,13 +1502,13 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E31">
         <v>8</v>
@@ -1490,7 +1520,7 @@
         <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1498,13 +1528,13 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -1516,7 +1546,7 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1524,13 +1554,13 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E33">
         <v>10</v>
@@ -1542,7 +1572,7 @@
         <v>30</v>
       </c>
       <c r="H33" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1550,13 +1580,13 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E34">
         <v>8</v>
@@ -1568,7 +1598,7 @@
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1576,13 +1606,13 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E35">
         <v>50</v>
@@ -1594,7 +1624,7 @@
         <v>50</v>
       </c>
       <c r="H35" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1602,13 +1632,13 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E36">
         <v>8</v>
@@ -1620,7 +1650,7 @@
         <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1631,10 +1661,10 @@
         <v>46002</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E37">
         <v>20</v>
@@ -1646,7 +1676,7 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1657,10 +1687,10 @@
         <v>46002</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E38">
         <v>8</v>
@@ -1672,7 +1702,7 @@
         <v>8</v>
       </c>
       <c r="H38" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1680,13 +1710,13 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E39">
         <v>8</v>
@@ -1698,7 +1728,7 @@
         <v>8</v>
       </c>
       <c r="H39" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1709,10 +1739,10 @@
         <v>46001</v>
       </c>
       <c r="C40" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E40">
         <v>10</v>
@@ -1724,7 +1754,7 @@
         <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1732,13 +1762,13 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -1750,7 +1780,7 @@
         <v>10</v>
       </c>
       <c r="H41" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1758,13 +1788,13 @@
         <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -1776,7 +1806,7 @@
         <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1784,13 +1814,13 @@
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E43">
         <v>10</v>
@@ -1802,7 +1832,7 @@
         <v>10</v>
       </c>
       <c r="H43" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1810,13 +1840,13 @@
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D44" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E44">
         <v>20</v>
@@ -1828,7 +1858,7 @@
         <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1836,13 +1866,13 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E45">
         <v>15</v>
@@ -1854,7 +1884,7 @@
         <v>15</v>
       </c>
       <c r="H45" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1862,13 +1892,13 @@
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -1880,7 +1910,7 @@
         <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1888,13 +1918,13 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E47">
         <v>15</v>
@@ -1906,7 +1936,7 @@
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1914,13 +1944,13 @@
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D48" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E48">
         <v>15</v>
@@ -1932,7 +1962,7 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1940,13 +1970,13 @@
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E49">
         <v>15</v>
@@ -1958,7 +1988,111 @@
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>101</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50">
+        <v>7</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>14</v>
+      </c>
+      <c r="H50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51">
+        <v>8</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>8</v>
+      </c>
+      <c r="H51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52">
+        <v>10</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>20</v>
+      </c>
+      <c r="H52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" t="s">
+        <v>108</v>
+      </c>
+      <c r="E53">
+        <v>15</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>15</v>
+      </c>
+      <c r="H53" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update in orders excel
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdace82c1c5d2c62/Documents/Devopslab/Harryskitchen/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_FFC65FC015E1ACC97249BB927110454A4B4ACA40" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3312F51E-817C-4112-AF41-05096ACA2AB0}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="111">
   <si>
     <t>Order ID</t>
   </si>
@@ -176,9 +182,6 @@
   </si>
   <si>
     <t>12/12/2025</t>
-  </si>
-  <si>
-    <t>12/16/2025</t>
   </si>
   <si>
     <t>Gowri</t>
@@ -355,11 +358,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,25 +414,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -467,7 +479,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -501,6 +513,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -535,9 +548,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -710,14 +724,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,7 +762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -751,10 +770,10 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -766,10 +785,10 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -777,10 +796,10 @@
         <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -792,10 +811,10 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -803,10 +822,10 @@
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -818,10 +837,10 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -829,10 +848,10 @@
         <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -844,10 +863,10 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -855,10 +874,10 @@
         <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -870,10 +889,10 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -881,10 +900,10 @@
         <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -896,10 +915,10 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -907,10 +926,10 @@
         <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -922,10 +941,10 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -933,10 +952,10 @@
         <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -948,10 +967,10 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -959,10 +978,10 @@
         <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -974,10 +993,10 @@
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -985,10 +1004,10 @@
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -1000,10 +1019,10 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1011,10 +1030,10 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -1026,10 +1045,10 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1037,10 +1056,10 @@
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13">
         <v>15</v>
@@ -1052,10 +1071,10 @@
         <v>45</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1063,10 +1082,10 @@
         <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -1078,10 +1097,10 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1089,10 +1108,10 @@
         <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -1104,10 +1123,10 @@
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1115,10 +1134,10 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -1130,10 +1149,10 @@
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1141,10 +1160,10 @@
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17">
         <v>20</v>
@@ -1156,10 +1175,10 @@
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1167,10 +1186,10 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -1182,10 +1201,10 @@
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1193,10 +1212,10 @@
         <v>45995</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19">
         <v>30</v>
@@ -1208,10 +1227,10 @@
         <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1219,10 +1238,10 @@
         <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20">
         <v>10</v>
@@ -1234,10 +1253,10 @@
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1245,10 +1264,10 @@
         <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21">
         <v>10</v>
@@ -1260,10 +1279,10 @@
         <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1271,10 +1290,10 @@
         <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -1286,10 +1305,10 @@
         <v>30</v>
       </c>
       <c r="H22" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1297,10 +1316,10 @@
         <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -1312,10 +1331,10 @@
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1323,10 +1342,10 @@
         <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E24">
         <v>10</v>
@@ -1338,10 +1357,10 @@
         <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1349,10 +1368,10 @@
         <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25">
         <v>80</v>
@@ -1364,10 +1383,10 @@
         <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1375,10 +1394,10 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26">
         <v>120</v>
@@ -1390,10 +1409,10 @@
         <v>120</v>
       </c>
       <c r="H26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1401,10 +1420,10 @@
         <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -1416,10 +1435,10 @@
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1427,10 +1446,10 @@
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E28">
         <v>20</v>
@@ -1442,10 +1461,10 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1453,10 +1472,10 @@
         <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1468,10 +1487,10 @@
         <v>30</v>
       </c>
       <c r="H29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1479,10 +1498,10 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -1494,10 +1513,10 @@
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1505,10 +1524,10 @@
         <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E31">
         <v>8</v>
@@ -1520,10 +1539,10 @@
         <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1531,10 +1550,10 @@
         <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -1546,10 +1565,10 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1557,10 +1576,10 @@
         <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E33">
         <v>10</v>
@@ -1572,10 +1591,10 @@
         <v>30</v>
       </c>
       <c r="H33" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1583,10 +1602,10 @@
         <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E34">
         <v>8</v>
@@ -1598,10 +1617,10 @@
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -1609,10 +1628,10 @@
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35">
         <v>50</v>
@@ -1624,10 +1643,10 @@
         <v>50</v>
       </c>
       <c r="H35" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -1635,10 +1654,10 @@
         <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36">
         <v>8</v>
@@ -1650,10 +1669,10 @@
         <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1661,10 +1680,10 @@
         <v>46002</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E37">
         <v>20</v>
@@ -1676,10 +1695,10 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1687,10 +1706,10 @@
         <v>46002</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38">
         <v>8</v>
@@ -1702,10 +1721,10 @@
         <v>8</v>
       </c>
       <c r="H38" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -1713,10 +1732,10 @@
         <v>53</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E39">
         <v>8</v>
@@ -1728,10 +1747,10 @@
         <v>8</v>
       </c>
       <c r="H39" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1739,10 +1758,10 @@
         <v>46001</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E40">
         <v>10</v>
@@ -1754,10 +1773,10 @@
         <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -1765,10 +1784,10 @@
         <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -1780,10 +1799,10 @@
         <v>10</v>
       </c>
       <c r="H41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -1791,10 +1810,10 @@
         <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -1806,10 +1825,10 @@
         <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1817,10 +1836,10 @@
         <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E43">
         <v>10</v>
@@ -1832,10 +1851,10 @@
         <v>10</v>
       </c>
       <c r="H43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1843,10 +1862,10 @@
         <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E44">
         <v>20</v>
@@ -1858,10 +1877,10 @@
         <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1869,10 +1888,10 @@
         <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E45">
         <v>15</v>
@@ -1884,10 +1903,10 @@
         <v>15</v>
       </c>
       <c r="H45" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -1895,10 +1914,10 @@
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -1910,10 +1929,10 @@
         <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1921,10 +1940,10 @@
         <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E47">
         <v>15</v>
@@ -1936,10 +1955,10 @@
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -1947,10 +1966,10 @@
         <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E48">
         <v>15</v>
@@ -1962,10 +1981,10 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -1973,10 +1992,10 @@
         <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E49">
         <v>15</v>
@@ -1988,21 +2007,21 @@
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>42</v>
       </c>
-      <c r="B50" t="s">
-        <v>54</v>
+      <c r="B50" s="3">
+        <v>46006</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -2014,21 +2033,21 @@
         <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>43</v>
       </c>
-      <c r="B51" t="s">
-        <v>54</v>
+      <c r="B51" s="3">
+        <v>46006</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E51">
         <v>8</v>
@@ -2040,21 +2059,21 @@
         <v>8</v>
       </c>
       <c r="H51" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>44</v>
       </c>
-      <c r="B52" t="s">
-        <v>54</v>
+      <c r="B52" s="3">
+        <v>46006</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E52">
         <v>10</v>
@@ -2066,21 +2085,21 @@
         <v>20</v>
       </c>
       <c r="H52" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>45</v>
       </c>
-      <c r="B53" t="s">
-        <v>54</v>
+      <c r="B53" s="3">
+        <v>46006</v>
       </c>
       <c r="C53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E53">
         <v>15</v>
@@ -2092,7 +2111,7 @@
         <v>15</v>
       </c>
       <c r="H53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to the session object to fix issues with addorders page
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdace82c1c5d2c62/Documents/Devopslab/Harryskitchen/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_23F921ED83D34F697765405651A096DD65F6992C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE6DCB53-5F24-4E2B-B60F-C4A040D38323}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="111">
   <si>
     <t>Order ID</t>
   </si>
@@ -154,12 +160,6 @@
     <t>HK1037</t>
   </si>
   <si>
-    <t>HK1038</t>
-  </si>
-  <si>
-    <t>HK1039</t>
-  </si>
-  <si>
     <t>12/03/2025</t>
   </si>
   <si>
@@ -184,9 +184,6 @@
     <t>12/12/2025</t>
   </si>
   <si>
-    <t>12/16/2025</t>
-  </si>
-  <si>
     <t>Gowri</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
     <t>Shalini Raju</t>
   </si>
   <si>
-    <t>Shalini</t>
-  </si>
-  <si>
     <t>Dosa Batter with Chutney</t>
   </si>
   <si>
@@ -350,12 +344,6 @@
   </si>
   <si>
     <t>Boiled egg curry with Jeera rice</t>
-  </si>
-  <si>
-    <t>Veg curries</t>
-  </si>
-  <si>
-    <t>Daily subscription</t>
   </si>
   <si>
     <t>Delivered</t>
@@ -370,11 +358,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,13 +426,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -482,7 +478,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -516,6 +512,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -550,9 +547,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -725,14 +723,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,18 +758,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -781,21 +781,21 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -807,21 +807,21 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -833,21 +833,21 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -859,21 +859,21 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -885,21 +885,21 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -911,21 +911,21 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -937,21 +937,21 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -963,21 +963,21 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -989,21 +989,21 @@
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -1015,21 +1015,21 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -1041,21 +1041,21 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E13">
         <v>15</v>
@@ -1067,21 +1067,21 @@
         <v>45</v>
       </c>
       <c r="H13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -1093,21 +1093,21 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -1119,21 +1119,21 @@
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -1145,21 +1145,21 @@
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E17">
         <v>20</v>
@@ -1171,21 +1171,21 @@
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -1197,10 +1197,10 @@
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1208,10 +1208,10 @@
         <v>45995</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E19">
         <v>30</v>
@@ -1223,21 +1223,21 @@
         <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E20">
         <v>10</v>
@@ -1249,21 +1249,21 @@
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E21">
         <v>10</v>
@@ -1275,21 +1275,21 @@
         <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -1301,21 +1301,21 @@
         <v>30</v>
       </c>
       <c r="H22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -1327,21 +1327,21 @@
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E24">
         <v>10</v>
@@ -1353,21 +1353,21 @@
         <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E25">
         <v>80</v>
@@ -1379,21 +1379,21 @@
         <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E26">
         <v>120</v>
@@ -1405,21 +1405,21 @@
         <v>120</v>
       </c>
       <c r="H26" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -1431,21 +1431,21 @@
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E28">
         <v>20</v>
@@ -1457,21 +1457,21 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1483,21 +1483,21 @@
         <v>30</v>
       </c>
       <c r="H29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -1509,21 +1509,21 @@
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E31">
         <v>8</v>
@@ -1535,21 +1535,21 @@
         <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -1561,21 +1561,21 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E33">
         <v>10</v>
@@ -1587,21 +1587,21 @@
         <v>30</v>
       </c>
       <c r="H33" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E34">
         <v>8</v>
@@ -1613,21 +1613,21 @@
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E35">
         <v>50</v>
@@ -1639,21 +1639,21 @@
         <v>50</v>
       </c>
       <c r="H35" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E36">
         <v>8</v>
@@ -1665,10 +1665,10 @@
         <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1676,10 +1676,10 @@
         <v>46002</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E37">
         <v>20</v>
@@ -1691,10 +1691,10 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1702,10 +1702,10 @@
         <v>46002</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E38">
         <v>8</v>
@@ -1717,21 +1717,21 @@
         <v>8</v>
       </c>
       <c r="H38" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
       <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
         <v>55</v>
       </c>
-      <c r="C39" t="s">
-        <v>58</v>
-      </c>
       <c r="D39" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E39">
         <v>8</v>
@@ -1743,10 +1743,10 @@
         <v>8</v>
       </c>
       <c r="H39" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1754,10 +1754,10 @@
         <v>46001</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D40" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E40">
         <v>10</v>
@@ -1769,21 +1769,21 @@
         <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D41" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -1795,21 +1795,21 @@
         <v>10</v>
       </c>
       <c r="H41" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -1821,21 +1821,21 @@
         <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E43">
         <v>10</v>
@@ -1847,21 +1847,21 @@
         <v>10</v>
       </c>
       <c r="H43" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E44">
         <v>20</v>
@@ -1873,21 +1873,21 @@
         <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E45">
         <v>15</v>
@@ -1899,21 +1899,21 @@
         <v>15</v>
       </c>
       <c r="H45" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -1925,21 +1925,21 @@
         <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E47">
         <v>15</v>
@@ -1951,21 +1951,21 @@
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E48">
         <v>15</v>
@@ -1977,21 +1977,21 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D49" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E49">
         <v>15</v>
@@ -2003,10 +2003,10 @@
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -2014,10 +2014,10 @@
         <v>46006</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -2029,10 +2029,10 @@
         <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -2040,10 +2040,10 @@
         <v>46006</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E51">
         <v>8</v>
@@ -2055,10 +2055,10 @@
         <v>8</v>
       </c>
       <c r="H51" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -2066,100 +2066,74 @@
         <v>46006</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D52" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E52">
         <v>10</v>
       </c>
       <c r="F52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G52">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H52" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" s="2">
         <v>46006</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D53" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="2">
+        <v>46006</v>
+      </c>
+      <c r="C54" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54">
         <v>15</v>
       </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53">
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
         <v>15</v>
       </c>
-      <c r="H53" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" t="s">
-        <v>46</v>
-      </c>
-      <c r="B54" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" t="s">
-        <v>77</v>
-      </c>
-      <c r="D54" t="s">
-        <v>112</v>
-      </c>
-      <c r="E54">
-        <v>10</v>
-      </c>
-      <c r="F54">
-        <v>2</v>
-      </c>
-      <c r="G54">
-        <v>20</v>
-      </c>
       <c r="H54" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" t="s">
-        <v>47</v>
-      </c>
-      <c r="B55" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" t="s">
-        <v>58</v>
-      </c>
-      <c r="D55" t="s">
-        <v>113</v>
-      </c>
-      <c r="E55">
-        <v>10</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55">
-        <v>10</v>
-      </c>
-      <c r="H55" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add gitignore and requirements file
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdace82c1c5d2c62/Documents/Devopslab/Harryskitchen/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_23F921ED83D34F697765405651A096DD65F6992C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE6DCB53-5F24-4E2B-B60F-C4A040D38323}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="117">
   <si>
     <t>Order ID</t>
   </si>
@@ -160,6 +154,18 @@
     <t>HK1037</t>
   </si>
   <si>
+    <t>HK1038</t>
+  </si>
+  <si>
+    <t>HK1039</t>
+  </si>
+  <si>
+    <t>HK1040</t>
+  </si>
+  <si>
+    <t>HK1041</t>
+  </si>
+  <si>
     <t>12/03/2025</t>
   </si>
   <si>
@@ -184,6 +190,9 @@
     <t>12/12/2025</t>
   </si>
   <si>
+    <t>12/17/2025</t>
+  </si>
+  <si>
     <t>Gowri</t>
   </si>
   <si>
@@ -344,6 +353,9 @@
   </si>
   <si>
     <t>Boiled egg curry with Jeera rice</t>
+  </si>
+  <si>
+    <t>Daily Veg Subscription</t>
   </si>
   <si>
     <t>Delivered</t>
@@ -358,11 +370,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,21 +438,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -478,7 +482,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -512,7 +516,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -547,10 +550,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -723,16 +725,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,18 +758,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -781,21 +781,21 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -807,21 +807,21 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -833,21 +833,21 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -859,21 +859,21 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -885,21 +885,21 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -911,21 +911,21 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -937,21 +937,21 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -963,21 +963,21 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -989,21 +989,21 @@
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -1015,21 +1015,21 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -1041,21 +1041,21 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E13">
         <v>15</v>
@@ -1067,21 +1067,21 @@
         <v>45</v>
       </c>
       <c r="H13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -1093,21 +1093,21 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -1119,21 +1119,21 @@
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -1145,21 +1145,21 @@
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E17">
         <v>20</v>
@@ -1171,21 +1171,21 @@
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -1197,10 +1197,10 @@
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1208,10 +1208,10 @@
         <v>45995</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E19">
         <v>30</v>
@@ -1223,21 +1223,21 @@
         <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E20">
         <v>10</v>
@@ -1249,21 +1249,21 @@
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E21">
         <v>10</v>
@@ -1275,21 +1275,21 @@
         <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -1301,21 +1301,21 @@
         <v>30</v>
       </c>
       <c r="H22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -1327,21 +1327,21 @@
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E24">
         <v>10</v>
@@ -1353,21 +1353,21 @@
         <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E25">
         <v>80</v>
@@ -1379,21 +1379,21 @@
         <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E26">
         <v>120</v>
@@ -1405,21 +1405,21 @@
         <v>120</v>
       </c>
       <c r="H26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -1431,21 +1431,21 @@
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E28">
         <v>20</v>
@@ -1457,21 +1457,21 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1483,21 +1483,21 @@
         <v>30</v>
       </c>
       <c r="H29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -1509,21 +1509,21 @@
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E31">
         <v>8</v>
@@ -1535,21 +1535,21 @@
         <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -1561,21 +1561,21 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E33">
         <v>10</v>
@@ -1587,21 +1587,21 @@
         <v>30</v>
       </c>
       <c r="H33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E34">
         <v>8</v>
@@ -1613,21 +1613,21 @@
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E35">
         <v>50</v>
@@ -1639,21 +1639,21 @@
         <v>50</v>
       </c>
       <c r="H35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E36">
         <v>8</v>
@@ -1665,10 +1665,10 @@
         <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1676,10 +1676,10 @@
         <v>46002</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E37">
         <v>20</v>
@@ -1691,10 +1691,10 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1702,10 +1702,10 @@
         <v>46002</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E38">
         <v>8</v>
@@ -1717,21 +1717,21 @@
         <v>8</v>
       </c>
       <c r="H38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E39">
         <v>8</v>
@@ -1743,10 +1743,10 @@
         <v>8</v>
       </c>
       <c r="H39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1754,10 +1754,10 @@
         <v>46001</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E40">
         <v>10</v>
@@ -1769,21 +1769,21 @@
         <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -1795,21 +1795,21 @@
         <v>10</v>
       </c>
       <c r="H41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -1821,21 +1821,21 @@
         <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E43">
         <v>10</v>
@@ -1847,21 +1847,21 @@
         <v>10</v>
       </c>
       <c r="H43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E44">
         <v>20</v>
@@ -1873,21 +1873,21 @@
         <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E45">
         <v>15</v>
@@ -1899,21 +1899,21 @@
         <v>15</v>
       </c>
       <c r="H45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -1925,21 +1925,21 @@
         <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E47">
         <v>15</v>
@@ -1951,21 +1951,21 @@
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E48">
         <v>15</v>
@@ -1977,21 +1977,21 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D49" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E49">
         <v>15</v>
@@ -2003,10 +2003,10 @@
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -2014,10 +2014,10 @@
         <v>46006</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D50" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -2029,10 +2029,10 @@
         <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -2040,10 +2040,10 @@
         <v>46006</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E51">
         <v>8</v>
@@ -2055,10 +2055,10 @@
         <v>8</v>
       </c>
       <c r="H51" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -2066,10 +2066,10 @@
         <v>46006</v>
       </c>
       <c r="C52" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D52" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E52">
         <v>10</v>
@@ -2081,10 +2081,10 @@
         <v>30</v>
       </c>
       <c r="H52" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>44</v>
       </c>
@@ -2092,10 +2092,10 @@
         <v>46006</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D53" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E53">
         <v>5</v>
@@ -2107,10 +2107,10 @@
         <v>5</v>
       </c>
       <c r="H53" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>45</v>
       </c>
@@ -2118,10 +2118,10 @@
         <v>46006</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D54" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E54">
         <v>15</v>
@@ -2133,7 +2133,111 @@
         <v>15</v>
       </c>
       <c r="H54" t="s">
-        <v>108</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>8</v>
+      </c>
+      <c r="H55" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56">
+        <v>15</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>30</v>
+      </c>
+      <c r="H56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" t="s">
+        <v>79</v>
+      </c>
+      <c r="E57">
+        <v>10</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>10</v>
+      </c>
+      <c r="H57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>8</v>
+      </c>
+      <c r="H58" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>